<commit_message>
2024.12.10. - hopefully végleges
</commit_message>
<xml_diff>
--- a/res/f1_time_thai_25.xlsx
+++ b/res/f1_time_thai_25.xlsx
@@ -460,10 +460,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.717948717948718</v>
+        <v>0.6842105263157895</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7724137931034482</v>
+        <v>0.7194244604316546</v>
       </c>
     </row>
     <row r="3">
@@ -476,10 +476,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.6086956521739131</v>
+        <v>0.6530612244897959</v>
       </c>
       <c r="D3" t="n">
-        <v>0.738255033557047</v>
+        <v>0.7862068965517242</v>
       </c>
     </row>
     <row r="4">
@@ -492,10 +492,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.5581395348837208</v>
+        <v>0.6222222222222222</v>
       </c>
       <c r="D4" t="n">
-        <v>0.6394557823129252</v>
+        <v>0.6754966887417219</v>
       </c>
     </row>
     <row r="5">
@@ -508,10 +508,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.5714285714285714</v>
+        <v>0.6341463414634146</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6901408450704226</v>
+        <v>0.676470588235294</v>
       </c>
     </row>
     <row r="6">
@@ -716,10 +716,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.7500000000000001</v>
+        <v>0.6500000000000001</v>
       </c>
       <c r="D18" t="n">
-        <v>0.7837837837837838</v>
+        <v>0.6950354609929078</v>
       </c>
     </row>
     <row r="19">
@@ -732,10 +732,10 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.7500000000000001</v>
+        <v>0.6500000000000001</v>
       </c>
       <c r="D19" t="n">
-        <v>0.7837837837837838</v>
+        <v>0.6950354609929078</v>
       </c>
     </row>
     <row r="20">
@@ -748,10 +748,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.7500000000000001</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="D20" t="n">
-        <v>0.7837837837837838</v>
+        <v>0.6950354609929078</v>
       </c>
     </row>
     <row r="21">
@@ -764,10 +764,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.5777777777777778</v>
+        <v>0.6808510638297872</v>
       </c>
       <c r="D21" t="n">
-        <v>0.7464788732394366</v>
+        <v>0.7808219178082192</v>
       </c>
     </row>
     <row r="22">
@@ -780,10 +780,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.5777777777777778</v>
+        <v>0.6808510638297872</v>
       </c>
       <c r="D22" t="n">
-        <v>0.7464788732394366</v>
+        <v>0.7808219178082192</v>
       </c>
     </row>
     <row r="23">
@@ -796,10 +796,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.5777777777777778</v>
+        <v>0.6808510638297872</v>
       </c>
       <c r="D23" t="n">
-        <v>0.7464788732394366</v>
+        <v>0.7808219178082192</v>
       </c>
     </row>
     <row r="24">
@@ -812,10 +812,10 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.5909090909090909</v>
+        <v>0.6046511627906977</v>
       </c>
       <c r="D24" t="n">
-        <v>0.7605633802816901</v>
+        <v>0.7866666666666666</v>
       </c>
     </row>
     <row r="25">
@@ -828,10 +828,10 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.5909090909090909</v>
+        <v>0.6046511627906977</v>
       </c>
       <c r="D25" t="n">
-        <v>0.7605633802816901</v>
+        <v>0.7866666666666666</v>
       </c>
     </row>
     <row r="26">
@@ -844,10 +844,10 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.5909090909090909</v>
+        <v>0.6046511627906977</v>
       </c>
       <c r="D26" t="n">
-        <v>0.7605633802816901</v>
+        <v>0.7866666666666666</v>
       </c>
     </row>
     <row r="27">
@@ -860,10 +860,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.7826086956521739</v>
+        <v>0.717948717948718</v>
       </c>
       <c r="D27" t="n">
-        <v>0.7785234899328859</v>
+        <v>0.72992700729927</v>
       </c>
     </row>
     <row r="28">
@@ -876,10 +876,10 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.7826086956521739</v>
+        <v>0.717948717948718</v>
       </c>
       <c r="D28" t="n">
-        <v>0.7785234899328859</v>
+        <v>0.72992700729927</v>
       </c>
     </row>
     <row r="29">
@@ -892,10 +892,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.7826086956521739</v>
+        <v>0.717948717948718</v>
       </c>
       <c r="D29" t="n">
-        <v>0.7785234899328859</v>
+        <v>0.72992700729927</v>
       </c>
     </row>
     <row r="30">
@@ -1580,7 +1580,7 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>0.6829268292682926</v>
+        <v>0.7272727272727272</v>
       </c>
       <c r="D72" t="n">
         <v>1</v>
@@ -1596,7 +1596,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>0.7441860465116279</v>
+        <v>0.7111111111111111</v>
       </c>
       <c r="D73" t="n">
         <v>1</v>
@@ -1612,7 +1612,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>0.5128205128205129</v>
+        <v>0.6521739130434783</v>
       </c>
       <c r="D74" t="n">
         <v>1</v>
@@ -1628,7 +1628,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>0.6818181818181819</v>
+        <v>0.6511627906976744</v>
       </c>
       <c r="D75" t="n">
         <v>1</v>
@@ -1772,10 +1772,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>0.6315789473684211</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="D84" t="n">
-        <v>0.8493150684931507</v>
+        <v>0.7638888888888888</v>
       </c>
     </row>
     <row r="85">
@@ -1788,10 +1788,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.6486486486486486</v>
       </c>
       <c r="D85" t="n">
-        <v>0.7536231884057971</v>
+        <v>0.7916666666666666</v>
       </c>
     </row>
     <row r="86">
@@ -1804,10 +1804,10 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>0.6486486486486486</v>
+        <v>0.6500000000000001</v>
       </c>
       <c r="D86" t="n">
-        <v>0.6962962962962963</v>
+        <v>0.7605633802816901</v>
       </c>
     </row>
     <row r="87">
@@ -1820,10 +1820,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>0.7142857142857143</v>
+        <v>0.717948717948718</v>
       </c>
       <c r="D87" t="n">
-        <v>0.7445255474452555</v>
+        <v>0.7076923076923075</v>
       </c>
     </row>
     <row r="88">
@@ -2156,10 +2156,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>0.6956521739130435</v>
+        <v>0.6486486486486486</v>
       </c>
       <c r="D108" t="n">
-        <v>0.9605263157894737</v>
+        <v>0.951048951048951</v>
       </c>
     </row>
     <row r="109">
@@ -2172,7 +2172,7 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>0.6976744186046512</v>
+        <v>0.5789473684210527</v>
       </c>
       <c r="D109" t="n">
         <v>0.943661971830986</v>
@@ -2188,10 +2188,10 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>0.6363636363636365</v>
+        <v>0.5116279069767442</v>
       </c>
       <c r="D110" t="n">
-        <v>0.9379310344827587</v>
+        <v>0.9733333333333333</v>
       </c>
     </row>
     <row r="111">
@@ -2204,10 +2204,10 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>0.6976744186046512</v>
+        <v>0.717948717948718</v>
       </c>
       <c r="D111" t="n">
-        <v>0.9517241379310345</v>
+        <v>0.9295774647887325</v>
       </c>
     </row>
     <row r="112">
@@ -2412,10 +2412,10 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.6153846153846153</v>
       </c>
       <c r="D124" t="n">
-        <v>0.6711409395973154</v>
+        <v>0.676056338028169</v>
       </c>
     </row>
     <row r="125">
@@ -2428,10 +2428,10 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>0.588235294117647</v>
+        <v>0.7567567567567567</v>
       </c>
       <c r="D125" t="n">
-        <v>0.6818181818181819</v>
+        <v>0.6870229007633588</v>
       </c>
     </row>
     <row r="126">
@@ -2447,7 +2447,7 @@
         <v>0.6976744186046512</v>
       </c>
       <c r="D126" t="n">
-        <v>0.6794871794871794</v>
+        <v>0.6493506493506493</v>
       </c>
     </row>
     <row r="127">
@@ -2460,10 +2460,10 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>0.7555555555555556</v>
+        <v>0.7441860465116279</v>
       </c>
       <c r="D127" t="n">
-        <v>0.6962025316455696</v>
+        <v>0.6979865771812082</v>
       </c>
     </row>
     <row r="128">
@@ -2671,7 +2671,7 @@
         <v>0.6666666666666666</v>
       </c>
       <c r="D140" t="n">
-        <v>0.8270676691729323</v>
+        <v>0.8609271523178808</v>
       </c>
     </row>
     <row r="141">
@@ -2684,10 +2684,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>0.6341463414634146</v>
+        <v>0.5641025641025642</v>
       </c>
       <c r="D141" t="n">
-        <v>0.8413793103448276</v>
+        <v>0.8918918918918919</v>
       </c>
     </row>
     <row r="142">
@@ -2700,10 +2700,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>0.7272727272727272</v>
+        <v>0.7441860465116279</v>
       </c>
       <c r="D142" t="n">
-        <v>0.8717948717948718</v>
+        <v>0.8588957055214724</v>
       </c>
     </row>
     <row r="143">
@@ -2716,10 +2716,10 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>0.7555555555555556</v>
+        <v>0.7368421052631577</v>
       </c>
       <c r="D143" t="n">
-        <v>0.8456375838926175</v>
+        <v>0.8000000000000002</v>
       </c>
     </row>
     <row r="144">
@@ -2924,10 +2924,10 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>0.5714285714285714</v>
+        <v>0.6500000000000001</v>
       </c>
       <c r="D156" t="n">
-        <v>0.7680000000000001</v>
+        <v>0.8311688311688312</v>
       </c>
     </row>
     <row r="157">
@@ -2940,10 +2940,10 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>0.611111111111111</v>
+        <v>0.5405405405405405</v>
       </c>
       <c r="D157" t="n">
-        <v>0.8088235294117647</v>
+        <v>0.8489208633093526</v>
       </c>
     </row>
     <row r="158">
@@ -2956,10 +2956,10 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.6956521739130435</v>
       </c>
       <c r="D158" t="n">
-        <v>0.85</v>
+        <v>0.8181818181818183</v>
       </c>
     </row>
     <row r="159">
@@ -2972,10 +2972,10 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>0.7619047619047619</v>
+        <v>0.7222222222222222</v>
       </c>
       <c r="D159" t="n">
-        <v>0.8201438848920863</v>
+        <v>0.7419354838709677</v>
       </c>
     </row>
     <row r="160">

</xml_diff>